<commit_message>
Added files to attempt adaptive filter on image
</commit_message>
<xml_diff>
--- a/LMSAdaptiveFilter.xlsx
+++ b/LMSAdaptiveFilter.xlsx
@@ -28,10 +28,10 @@
     <t>estimated y protein</t>
   </si>
   <si>
-    <t>estimated a1</t>
+    <t>estimated a</t>
   </si>
   <si>
-    <t>estimated b1</t>
+    <t>estimated b</t>
   </si>
   <si>
     <t>y protein estimation error</t>
@@ -400,10 +400,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>5.021760936599735</v>
+        <v>5.06425973678165</v>
       </c>
       <c r="C2">
-        <v>-0.007544587694176839</v>
+        <v>0.2659740790387403</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -423,10 +423,10 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>5.111135417788932</v>
+        <v>4.719634038318971</v>
       </c>
       <c r="C3">
-        <v>1.0406608768353</v>
+        <v>1.123697297921999</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -438,7 +438,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>1.0406608768353</v>
+        <v>1.123697297921999</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -446,22 +446,22 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>5.089400520026556</v>
+        <v>4.848420907460548</v>
       </c>
       <c r="C4">
-        <v>1.399668094021833</v>
+        <v>2.051514153718679</v>
       </c>
       <c r="D4">
-        <v>0.02670236824948238</v>
+        <v>0.02719384204359941</v>
       </c>
       <c r="E4">
-        <v>0.005225950139539138</v>
+        <v>0.005690694982196712</v>
       </c>
       <c r="F4">
-        <v>-7.851357245182883E-06</v>
+        <v>0.0002988743539331245</v>
       </c>
       <c r="G4">
-        <v>1.372965725772351</v>
+        <v>2.024320311675079</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -469,22 +469,22 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>4.637483127740302</v>
+        <v>5.058314096757192</v>
       </c>
       <c r="C5">
-        <v>1.966336566576342</v>
+        <v>3.088031821506794</v>
       </c>
       <c r="D5">
-        <v>0.06430022742190195</v>
+        <v>0.07919271731892807</v>
       </c>
       <c r="E5">
-        <v>0.01224336388794449</v>
+        <v>0.01524474602963889</v>
       </c>
       <c r="F5">
-        <v>0.001420940358801886</v>
+        <v>0.002573597618291029</v>
       </c>
       <c r="G5">
-        <v>1.90203633915444</v>
+        <v>3.008839104187865</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -492,22 +492,22 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>4.624905457916486</v>
+        <v>5.383498241494825</v>
       </c>
       <c r="C6">
-        <v>2.625208813379272</v>
+        <v>3.759761072173697</v>
       </c>
       <c r="D6">
-        <v>0.1096991390220374</v>
+        <v>0.1779127700710449</v>
       </c>
       <c r="E6">
-        <v>0.0219235886215465</v>
+        <v>0.0298328644495682</v>
       </c>
       <c r="F6">
-        <v>0.004083159936386447</v>
+        <v>0.008746273626794665</v>
       </c>
       <c r="G6">
-        <v>2.515509674357234</v>
+        <v>3.581848302102653</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -515,22 +515,22 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>4.503001273893294</v>
+        <v>5.629808561203252</v>
       </c>
       <c r="C7">
-        <v>3.262361366700904</v>
+        <v>4.604997168059289</v>
       </c>
       <c r="D7">
-        <v>0.1790512968007268</v>
+        <v>0.3326141026026326</v>
       </c>
       <c r="E7">
-        <v>0.03358922229404568</v>
+        <v>0.04795097820853986</v>
       </c>
       <c r="F7">
-        <v>0.009029498592651623</v>
+        <v>0.01980713516349774</v>
       </c>
       <c r="G7">
-        <v>3.083310069900177</v>
+        <v>4.272383065456657</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -538,22 +538,22 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>4.713874275200235</v>
+        <v>5.592776040936967</v>
       </c>
       <c r="C8">
-        <v>3.698693868898403</v>
+        <v>5.412585458791135</v>
       </c>
       <c r="D8">
-        <v>0.2713293139529458</v>
+        <v>0.5646250025106063</v>
       </c>
       <c r="E8">
-        <v>0.04784923986477587</v>
+        <v>0.07095134492841804</v>
       </c>
       <c r="F8">
-        <v>0.01712383136253463</v>
+        <v>0.0358702746984158</v>
       </c>
       <c r="G8">
-        <v>3.427364554945457</v>
+        <v>4.847960456280529</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -561,22 +561,22 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>4.790021832574938</v>
+        <v>5.410445612584827</v>
       </c>
       <c r="C9">
-        <v>4.013926917942603</v>
+        <v>5.850246094395676</v>
       </c>
       <c r="D9">
-        <v>0.4029985573645653</v>
+        <v>0.8644451719734658</v>
       </c>
       <c r="E9">
-        <v>0.06328266682179198</v>
+        <v>0.09824443420956097</v>
       </c>
       <c r="F9">
-        <v>0.02830513307618873</v>
+        <v>0.05819511887045106</v>
       </c>
       <c r="G9">
-        <v>3.610928360578038</v>
+        <v>4.985800922422211</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -584,22 +584,22 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>4.682164321179759</v>
+        <v>5.389353871293725</v>
       </c>
       <c r="C10">
-        <v>4.366838884114461</v>
+        <v>6.373146445832048</v>
       </c>
       <c r="D10">
-        <v>0.551882145700621</v>
+        <v>1.180744503684842</v>
       </c>
       <c r="E10">
-        <v>0.08030412913031175</v>
+        <v>0.1261289021533653</v>
       </c>
       <c r="F10">
-        <v>0.04166085166449008</v>
+        <v>0.08518119244358094</v>
       </c>
       <c r="G10">
-        <v>3.81495673841384</v>
+        <v>5.192401942147206</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -607,22 +607,22 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>4.681261384699176</v>
+        <v>5.313964789347017</v>
       </c>
       <c r="C11">
-        <v>4.893858166840394</v>
+        <v>6.901265691769639</v>
       </c>
       <c r="D11">
-        <v>0.7103531618886767</v>
+        <v>1.567625722861011</v>
       </c>
       <c r="E11">
-        <v>0.09857785519764292</v>
+        <v>0.1542221104600326</v>
       </c>
       <c r="F11">
-        <v>0.05697380920759591</v>
+        <v>0.1155580216261602</v>
       </c>
       <c r="G11">
-        <v>4.183505004951718</v>
+        <v>5.333639968908629</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -630,22 +630,22 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>5.002089596582427</v>
+        <v>5.567358761293055</v>
       </c>
       <c r="C12">
-        <v>5.395148307905994</v>
+        <v>7.429004723453094</v>
       </c>
       <c r="D12">
-        <v>0.9213907202178613</v>
+        <v>2.00436501581576</v>
       </c>
       <c r="E12">
-        <v>0.1181657130693048</v>
+        <v>0.1829669836745573</v>
       </c>
       <c r="F12">
-        <v>0.07524250153510653</v>
+        <v>0.1495500902373579</v>
       </c>
       <c r="G12">
-        <v>4.473757587688133</v>
+        <v>5.424639707637334</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -653,22 +653,22 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>5.101982958860686</v>
+        <v>5.638730409950629</v>
       </c>
       <c r="C13">
-        <v>5.933016296074032</v>
+        <v>7.704836670351932</v>
       </c>
       <c r="D13">
-        <v>1.219898871064139</v>
+        <v>2.568256525054678</v>
       </c>
       <c r="E13">
-        <v>0.1391085417090542</v>
+        <v>0.2117933280758358</v>
       </c>
       <c r="F13">
-        <v>0.09713643664207827</v>
+        <v>0.1869869701418868</v>
       </c>
       <c r="G13">
-        <v>4.713117425009894</v>
+        <v>5.136580145297255</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -676,22 +676,22 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>4.47717576908199</v>
+        <v>5.734659041911391</v>
       </c>
       <c r="C14">
-        <v>6.236722007244168</v>
+        <v>7.870524098650011</v>
       </c>
       <c r="D14">
-        <v>1.557187487206575</v>
+        <v>3.090215445441184</v>
       </c>
       <c r="E14">
-        <v>0.1626839773481676</v>
+        <v>0.2403905125508404</v>
       </c>
       <c r="F14">
-        <v>0.1225644041425827</v>
+        <v>0.2251466483036954</v>
       </c>
       <c r="G14">
-        <v>4.679534520037593</v>
+        <v>4.780308653208827</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -699,22 +699,22 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>4.224150126326825</v>
+        <v>5.490575916791897</v>
       </c>
       <c r="C15">
-        <v>6.606382522990822</v>
+        <v>8.068690001250731</v>
       </c>
       <c r="D15">
-        <v>1.772811844965201</v>
+        <v>3.595039934653543</v>
       </c>
       <c r="E15">
-        <v>0.1865588827247997</v>
+        <v>0.2673453843226391</v>
       </c>
       <c r="F15">
-        <v>0.1503281587080067</v>
+        <v>0.2619781457105395</v>
       </c>
       <c r="G15">
-        <v>4.833570678025621</v>
+        <v>4.473650066597188</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -722,22 +722,22 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>4.107216206207418</v>
+        <v>5.471274035358311</v>
       </c>
       <c r="C16">
-        <v>6.519394366551912</v>
+        <v>8.321240740255618</v>
       </c>
       <c r="D16">
-        <v>2.071745413262958</v>
+        <v>4.006658856072908</v>
       </c>
       <c r="E16">
-        <v>0.2081996282426012</v>
+        <v>0.2930002421273982</v>
       </c>
       <c r="F16">
-        <v>0.1804737953292192</v>
+        <v>0.2971881163686199</v>
       </c>
       <c r="G16">
-        <v>4.447648953288954</v>
+        <v>4.31458188418271</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -745,22 +745,22 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>4.253923251282201</v>
+        <v>5.564644278991391</v>
       </c>
       <c r="C17">
-        <v>6.554756282476843</v>
+        <v>8.721742271392683</v>
       </c>
       <c r="D17">
-        <v>2.300423726998947</v>
+        <v>4.495357991469259</v>
       </c>
       <c r="E17">
-        <v>0.2269871651304941</v>
+        <v>0.3166897815117183</v>
       </c>
       <c r="F17">
-        <v>0.2098566656426257</v>
+        <v>0.3320011400771025</v>
       </c>
       <c r="G17">
-        <v>4.254332555477896</v>
+        <v>4.226384279923424</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -768,22 +768,22 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>4.121850816112879</v>
+        <v>5.749919442404175</v>
       </c>
       <c r="C18">
-        <v>6.976081198464002</v>
+        <v>8.878635381502809</v>
       </c>
       <c r="D18">
-        <v>2.597276618494449</v>
+        <v>5.093302429880228</v>
       </c>
       <c r="E18">
-        <v>0.2444606287489487</v>
+        <v>0.3398134880859099</v>
       </c>
       <c r="F18">
-        <v>0.2375923373382467</v>
+        <v>0.3671699011311771</v>
       </c>
       <c r="G18">
-        <v>4.378804579969553</v>
+        <v>3.785332951622581</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -791,22 +791,22 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>4.005815521759716</v>
+        <v>5.657541647639578</v>
       </c>
       <c r="C19">
-        <v>7.11032654576329</v>
+        <v>8.92320678803148</v>
       </c>
       <c r="D19">
-        <v>2.942099261597302</v>
+        <v>5.628109810017568</v>
       </c>
       <c r="E19">
-        <v>0.2630877273645022</v>
+        <v>0.3608775194392341</v>
       </c>
       <c r="F19">
-        <v>0.2662943341685405</v>
+        <v>0.4001845995466394</v>
       </c>
       <c r="G19">
-        <v>4.168227284165988</v>
+        <v>3.295096978013913</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -814,22 +814,22 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>4.123980645013667</v>
+        <v>5.750398649076522</v>
       </c>
       <c r="C20">
-        <v>6.891867162484539</v>
+        <v>9.080991702819514</v>
       </c>
       <c r="D20">
-        <v>3.222897041895571</v>
+        <v>5.980857404556438</v>
       </c>
       <c r="E20">
-        <v>0.2802685383974858</v>
+        <v>0.3798240616177235</v>
       </c>
       <c r="F20">
-        <v>0.2953722261565356</v>
+        <v>0.4294405641611168</v>
       </c>
       <c r="G20">
-        <v>3.668970120588968</v>
+        <v>3.100134298263076</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -837,22 +837,22 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>4.07430551090704</v>
+        <v>6.069971217198903</v>
       </c>
       <c r="C21">
-        <v>7.277230461243658</v>
+        <v>9.176774439685465</v>
       </c>
       <c r="D21">
-        <v>3.431891320177701</v>
+        <v>6.435951750976958</v>
       </c>
       <c r="E21">
-        <v>0.2949657558554137</v>
+        <v>0.3973632005234228</v>
       </c>
       <c r="F21">
-        <v>0.3214598018005717</v>
+        <v>0.457103703575187</v>
       </c>
       <c r="G21">
-        <v>3.845339141065957</v>
+        <v>2.740822688708507</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -860,22 +860,22 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>4.039520667030494</v>
+        <v>6.205585331465035</v>
       </c>
       <c r="C22">
-        <v>7.735012876204277</v>
+        <v>9.515790005205892</v>
       </c>
       <c r="D22">
-        <v>3.798586435042274</v>
+        <v>6.930792816190187</v>
       </c>
       <c r="E22">
-        <v>0.3108238600466832</v>
+        <v>0.4131240236099304</v>
       </c>
       <c r="F22">
-        <v>0.3479613683555006</v>
+        <v>0.4819930916702485</v>
       </c>
       <c r="G22">
-        <v>3.936426441162004</v>
+        <v>2.584997189015705</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -883,22 +883,22 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>3.977886239859078</v>
+        <v>6.289838851056939</v>
       </c>
       <c r="C23">
-        <v>7.606909497531193</v>
+        <v>9.760254810321053</v>
       </c>
       <c r="D23">
-        <v>4.233431090670361</v>
+        <v>7.473325349577257</v>
       </c>
       <c r="E23">
-        <v>0.3268620639891897</v>
+        <v>0.4288148821437959</v>
       </c>
       <c r="F23">
-        <v>0.3766076507615697</v>
+        <v>0.5057150278010666</v>
       </c>
       <c r="G23">
-        <v>3.373478406860832</v>
+        <v>2.286929460743796</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -906,22 +906,22 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>3.792201434645084</v>
+        <v>6.107574737100685</v>
       </c>
       <c r="C24">
-        <v>8.020972029090206</v>
+        <v>10.03814414871607</v>
       </c>
       <c r="D24">
-        <v>4.417741943131768</v>
+        <v>7.934749854790259</v>
       </c>
       <c r="E24">
-        <v>0.3404892997334851</v>
+        <v>0.4430066180594828</v>
       </c>
       <c r="F24">
-        <v>0.4027015496762353</v>
+        <v>0.5274769683062233</v>
       </c>
       <c r="G24">
-        <v>3.603230085958439</v>
+        <v>2.103394293925814</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -929,22 +929,22 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>3.865606796717036</v>
+        <v>6.13217816392083</v>
       </c>
       <c r="C25">
-        <v>7.851200620223572</v>
+        <v>10.46344736274409</v>
       </c>
       <c r="D25">
-        <v>4.795466800869911</v>
+        <v>8.28746888299959</v>
       </c>
       <c r="E25">
-        <v>0.3548225391114654</v>
+        <v>0.4562366292085089</v>
       </c>
       <c r="F25">
-        <v>0.4301109948389027</v>
+        <v>0.5480066325815145</v>
       </c>
       <c r="G25">
-        <v>3.055733819353661</v>
+        <v>2.175978479744495</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -952,22 +952,22 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>3.789536260011062</v>
+        <v>6.061523393111076</v>
       </c>
       <c r="C26">
-        <v>7.803795073297094</v>
+        <v>10.85185028680624</v>
       </c>
       <c r="D26">
-        <v>4.98571919590925</v>
+        <v>8.841810036003395</v>
       </c>
       <c r="E26">
-        <v>0.3664104972851119</v>
+        <v>0.4695265803998711</v>
       </c>
       <c r="F26">
-        <v>0.4546209503322834</v>
+        <v>0.5698494182256938</v>
       </c>
       <c r="G26">
-        <v>2.818075877387844</v>
+        <v>2.010040250802849</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -975,22 +975,22 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>4.196468821232549</v>
+        <v>6.174473733152114</v>
       </c>
       <c r="C27">
-        <v>7.810760285029305</v>
+        <v>10.88931745412158</v>
       </c>
       <c r="D27">
-        <v>5.150237332672867</v>
+        <v>9.33291638228286</v>
       </c>
       <c r="E27">
-        <v>0.3773040705504067</v>
+        <v>0.4818525053344463</v>
       </c>
       <c r="F27">
-        <v>0.4767462294086679</v>
+        <v>0.5908813685869663</v>
       </c>
       <c r="G27">
-        <v>2.660522952356438</v>
+        <v>1.556401071838717</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -998,22 +998,22 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>4.423074451414518</v>
+        <v>6.074148994337723</v>
       </c>
       <c r="C28">
-        <v>7.650044403224269</v>
+        <v>10.98376403362054</v>
       </c>
       <c r="D28">
-        <v>5.51157308247079</v>
+        <v>9.651650156178793</v>
       </c>
       <c r="E28">
-        <v>0.3873862187489531</v>
+        <v>0.4912866668404599</v>
       </c>
       <c r="F28">
-        <v>0.4975084053166609</v>
+        <v>0.6077712000047848</v>
       </c>
       <c r="G28">
-        <v>2.138471320753479</v>
+        <v>1.332113877441744</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1021,22 +1021,22 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>3.979213275465499</v>
+        <v>6.236960002928363</v>
       </c>
       <c r="C29">
-        <v>7.726765333470625</v>
+        <v>11.14444529651158</v>
       </c>
       <c r="D29">
-        <v>5.686871629757614</v>
+        <v>9.869052760534409</v>
       </c>
       <c r="E29">
-        <v>0.3963602469715951</v>
+        <v>0.4995117689862913</v>
       </c>
       <c r="F29">
-        <v>0.5142114921794764</v>
+        <v>0.6222770109012887</v>
       </c>
       <c r="G29">
-        <v>2.039893703713011</v>
+        <v>1.275392535977172</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1044,22 +1044,22 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>4.099369764171307</v>
+        <v>6.495994508525466</v>
       </c>
       <c r="C30">
-        <v>7.609107749656752</v>
+        <v>11.3639326725116</v>
       </c>
       <c r="D30">
-        <v>5.706874661542613</v>
+        <v>10.25480248360762</v>
       </c>
       <c r="E30">
-        <v>0.4053828486960894</v>
+        <v>0.5072586932760829</v>
       </c>
       <c r="F30">
-        <v>0.5298167695907385</v>
+        <v>0.6362856215667029</v>
       </c>
       <c r="G30">
-        <v>1.902233088114139</v>
+        <v>1.109130188903977</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1067,22 +1067,22 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>3.961518660407594</v>
+        <v>6.425142746759602</v>
       </c>
       <c r="C31">
-        <v>7.488103656840964</v>
+        <v>11.54131738845568</v>
       </c>
       <c r="D31">
-        <v>5.836116306165704</v>
+        <v>10.71125883447116</v>
       </c>
       <c r="E31">
-        <v>0.412952239853343</v>
+        <v>0.5141762939023173</v>
       </c>
       <c r="F31">
-        <v>0.5445148782721596</v>
+        <v>0.6486462622836529</v>
       </c>
       <c r="G31">
-        <v>1.65198735067526</v>
+        <v>0.8300585539845216</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1090,22 +1090,22 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>3.749050943744785</v>
+        <v>6.641519267546751</v>
       </c>
       <c r="C32">
-        <v>7.455223790222731</v>
+        <v>11.63331319779513</v>
       </c>
       <c r="D32">
-        <v>5.834256267793404</v>
+        <v>10.93339932469068</v>
       </c>
       <c r="E32">
-        <v>0.4197243468494946</v>
+        <v>0.5195683497107554</v>
       </c>
       <c r="F32">
-        <v>0.5570850280245176</v>
+        <v>0.6580789918053753</v>
       </c>
       <c r="G32">
-        <v>1.620967522429327</v>
+        <v>0.6999138731044532</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1113,22 +1113,22 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>3.962004086642852</v>
+        <v>6.645052895780783</v>
       </c>
       <c r="C33">
-        <v>7.562701225586099</v>
+        <v>11.82652128409962</v>
       </c>
       <c r="D33">
-        <v>5.841327321320542</v>
+        <v>11.23020251545492</v>
       </c>
       <c r="E33">
-        <v>0.426145839937513</v>
+        <v>0.5240653962558889</v>
       </c>
       <c r="F33">
-        <v>0.5692230008568411</v>
+        <v>0.6661569199594571</v>
       </c>
       <c r="G33">
-        <v>1.721373904265556</v>
+        <v>0.5963187686447053</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1136,22 +1136,22 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>3.645827076079204</v>
+        <v>6.790478226632451</v>
       </c>
       <c r="C34">
-        <v>7.627232678418025</v>
+        <v>11.64147642253117</v>
       </c>
       <c r="D34">
-        <v>6.115877778789201</v>
+        <v>11.46912126071904</v>
       </c>
       <c r="E34">
-        <v>0.4325993583978374</v>
+        <v>0.5280258588474425</v>
       </c>
       <c r="F34">
-        <v>0.5820562285397902</v>
+        <v>0.6730940829608245</v>
       </c>
       <c r="G34">
-        <v>1.511354899628824</v>
+        <v>0.172355161812126</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1159,22 +1159,22 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>3.905164324450834</v>
+        <v>7.105736027818379</v>
       </c>
       <c r="C35">
-        <v>7.580119458367746</v>
+        <v>11.96011989975266</v>
       </c>
       <c r="D35">
-        <v>6.125670634325858</v>
+        <v>11.45286373454056</v>
       </c>
       <c r="E35">
-        <v>0.4385873526865345</v>
+        <v>0.5291711680145449</v>
       </c>
       <c r="F35">
-        <v>0.5934861540915087</v>
+        <v>0.67513244495042</v>
       </c>
       <c r="G35">
-        <v>1.454448824041888</v>
+        <v>0.507256165212091</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1182,22 +1182,22 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>4.103107899875999</v>
+        <v>7.229207326483563</v>
       </c>
       <c r="C36">
-        <v>7.322090771054411</v>
+        <v>12.07087639181568</v>
       </c>
       <c r="D36">
-        <v>6.31624886696228</v>
+        <v>11.92991844374691</v>
       </c>
       <c r="E36">
-        <v>0.443890021589998</v>
+        <v>0.5326156799597427</v>
       </c>
       <c r="F36">
-        <v>0.6045795736913276</v>
+        <v>0.6810376556379202</v>
       </c>
       <c r="G36">
-        <v>1.00584190409213</v>
+        <v>0.140957948068765</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1205,22 +1205,22 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>3.666586089201576</v>
+        <v>7.40474599369551</v>
       </c>
       <c r="C37">
-        <v>7.4781005362455</v>
+        <v>12.00378460710251</v>
       </c>
       <c r="D37">
-        <v>6.320058650364883</v>
+        <v>12.09870135745569</v>
       </c>
       <c r="E37">
-        <v>0.4478179995098963</v>
+        <v>0.5336172899297422</v>
       </c>
       <c r="F37">
-        <v>0.612203975480578</v>
+        <v>0.6827235295976457</v>
       </c>
       <c r="G37">
-        <v>1.158041885880617</v>
+        <v>-0.09491675035317648</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1228,22 +1228,22 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>3.750912859111013</v>
+        <v>7.387780591782156</v>
       </c>
       <c r="C38">
-        <v>7.600307019194111</v>
+        <v>12.19560255487345</v>
       </c>
       <c r="D38">
-        <v>6.300917134947371</v>
+        <v>12.12773267301249</v>
       </c>
       <c r="E38">
-        <v>0.4525695703202404</v>
+        <v>0.532931117062683</v>
       </c>
       <c r="F38">
-        <v>0.6206832632856789</v>
+        <v>0.6815778012366197</v>
       </c>
       <c r="G38">
-        <v>1.29938988424674</v>
+        <v>0.06786988186096288</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1251,22 +1251,22 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>3.574468514032177</v>
+        <v>7.578205470017883</v>
       </c>
       <c r="C39">
-        <v>7.225233409094796</v>
+        <v>12.19649064650637</v>
       </c>
       <c r="D39">
-        <v>6.506654892579054</v>
+        <v>12.26307863669545</v>
       </c>
       <c r="E39">
-        <v>0.4573338951942687</v>
+        <v>0.5334336762984856</v>
       </c>
       <c r="F39">
-        <v>0.6304002314758564</v>
+        <v>0.6823924966797882</v>
       </c>
       <c r="G39">
-        <v>0.7185785165157421</v>
+        <v>-0.0665879901890829</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1274,22 +1274,22 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>3.833866548198694</v>
+        <v>7.404605160302087</v>
       </c>
       <c r="C40">
-        <v>7.137186500987511</v>
+        <v>12.52539023960694</v>
       </c>
       <c r="D40">
-        <v>6.2386087931489</v>
+        <v>12.35163116924213</v>
       </c>
       <c r="E40">
-        <v>0.4600292205921485</v>
+        <v>0.5329417388369209</v>
       </c>
       <c r="F40">
-        <v>0.6358616488187732</v>
+        <v>0.6815804160165143</v>
       </c>
       <c r="G40">
-        <v>0.8985777078386104</v>
+        <v>0.1737590703648113</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1297,22 +1297,22 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>4.023530959647532</v>
+        <v>7.362225443942344</v>
       </c>
       <c r="C41">
-        <v>7.145399416992959</v>
+        <v>12.70042992242894</v>
       </c>
       <c r="D41">
-        <v>6.360605667048631</v>
+        <v>12.51957853438532</v>
       </c>
       <c r="E41">
-        <v>0.4632411583162288</v>
+        <v>0.5342585207744247</v>
       </c>
       <c r="F41">
-        <v>0.6423540824941165</v>
+        <v>0.6836996668929644</v>
       </c>
       <c r="G41">
-        <v>0.7847937499443276</v>
+        <v>0.1808513880436173</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1320,22 +1320,22 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>4.414255546210933</v>
+        <v>6.970399004572669</v>
       </c>
       <c r="C42">
-        <v>7.016941806767295</v>
+        <v>13.00680590708403</v>
       </c>
       <c r="D42">
-        <v>6.505870556203774</v>
+        <v>12.65523983093785</v>
       </c>
       <c r="E42">
-        <v>0.4662499528213758</v>
+        <v>0.5355976538955802</v>
       </c>
       <c r="F42">
-        <v>0.6479553018522786</v>
+        <v>0.6859649011035852</v>
       </c>
       <c r="G42">
-        <v>0.5110712505635204</v>
+        <v>0.3515660761461863</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1343,22 +1343,22 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>4.466468096036707</v>
+        <v>6.953750103073991</v>
       </c>
       <c r="C43">
-        <v>6.991098764433922</v>
+        <v>13.13798911901098</v>
       </c>
       <c r="D43">
-        <v>6.63951269461907</v>
+        <v>12.7316591384756</v>
       </c>
       <c r="E43">
-        <v>0.4683062638206039</v>
+        <v>0.5381859626066107</v>
       </c>
       <c r="F43">
-        <v>0.651607110068097</v>
+        <v>0.6904299414167832</v>
       </c>
       <c r="G43">
-        <v>0.3515860698148519</v>
+        <v>0.4063299805353786</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1366,22 +1366,22 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>4.559643352307557</v>
+        <v>7.067791453856533</v>
       </c>
       <c r="C44">
-        <v>6.888546432321419</v>
+        <v>12.89725880043878</v>
       </c>
       <c r="D44">
-        <v>6.671304018901648</v>
+        <v>12.90240173020335</v>
       </c>
       <c r="E44">
-        <v>0.4698582545792546</v>
+        <v>0.5410182446984625</v>
       </c>
       <c r="F44">
-        <v>0.6540741690600579</v>
+        <v>0.6957149966078361</v>
       </c>
       <c r="G44">
-        <v>0.2172424134197701</v>
+        <v>-0.005142929764575754</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1389,22 +1389,22 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>4.553839219485256</v>
+        <v>7.098151070052287</v>
       </c>
       <c r="C45">
-        <v>7.170596800659393</v>
+        <v>13.14338509323391</v>
       </c>
       <c r="D45">
-        <v>6.662892672084059</v>
+        <v>12.79549628709082</v>
       </c>
       <c r="E45">
-        <v>0.4708285608879</v>
+        <v>0.5409824820500819</v>
       </c>
       <c r="F45">
-        <v>0.6555929322280994</v>
+        <v>0.6956474288525493</v>
       </c>
       <c r="G45">
-        <v>0.5077041285753339</v>
+        <v>0.3478888061430965</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -1412,22 +1412,22 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>4.751472481708299</v>
+        <v>7.167965481519667</v>
       </c>
       <c r="C46">
-        <v>7.331192582563526</v>
+        <v>13.46551932500427</v>
       </c>
       <c r="D46">
-        <v>6.880690097430075</v>
+        <v>13.05956230099899</v>
       </c>
       <c r="E46">
-        <v>0.4731435106426976</v>
+        <v>0.5434412875810325</v>
       </c>
       <c r="F46">
-        <v>0.6590902756916719</v>
+        <v>0.7001342408191524</v>
       </c>
       <c r="G46">
-        <v>0.4505024851334509</v>
+        <v>0.4059570240052874</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -1435,22 +1435,22 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>4.987753958307393</v>
+        <v>7.466889369872271</v>
       </c>
       <c r="C47">
-        <v>7.395272759112065</v>
+        <v>13.09648090534562</v>
       </c>
       <c r="D47">
-        <v>7.113476309271827</v>
+        <v>13.41554164184868</v>
       </c>
       <c r="E47">
-        <v>0.4751950265279739</v>
+        <v>0.5463228318653709</v>
       </c>
       <c r="F47">
-        <v>0.6623206473702589</v>
+        <v>0.7054698903169572</v>
       </c>
       <c r="G47">
-        <v>0.2817964498402379</v>
+        <v>-0.3190607365030687</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -1458,22 +1458,22 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>5.273703922450755</v>
+        <v>7.607095462784947</v>
       </c>
       <c r="C48">
-        <v>8.117240433015258</v>
+        <v>13.53483650461242</v>
       </c>
       <c r="D48">
-        <v>7.290153983289066</v>
+        <v>13.24516154219362</v>
       </c>
       <c r="E48">
-        <v>0.4765339746048329</v>
+        <v>0.5440358155196087</v>
       </c>
       <c r="F48">
-        <v>0.6643865514131203</v>
+        <v>0.701173571803725</v>
       </c>
       <c r="G48">
-        <v>0.8270864497261918</v>
+        <v>0.2896749624187986</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1481,22 +1481,22 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>5.254528364661137</v>
+        <v>7.65888999625207</v>
       </c>
       <c r="C49">
-        <v>8.097494702598251</v>
+        <v>13.61731994755215</v>
       </c>
       <c r="D49">
-        <v>7.977489443453518</v>
+        <v>13.6966033809769</v>
       </c>
       <c r="E49">
-        <v>0.4806592783183171</v>
+        <v>0.5461987864172118</v>
       </c>
       <c r="F49">
-        <v>0.6705030813042111</v>
+        <v>0.7049672944177995</v>
       </c>
       <c r="G49">
-        <v>0.1200052591447331</v>
+        <v>-0.07928343342474875</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -1504,22 +1504,22 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>5.25508570649307</v>
+        <v>8.067559439141933</v>
       </c>
       <c r="C50">
-        <v>7.923532530666908</v>
+        <v>13.49843848029324</v>
       </c>
       <c r="D50">
-        <v>7.966246268603422</v>
+        <v>13.7638098310167</v>
       </c>
       <c r="E50">
-        <v>0.4812921505241834</v>
+        <v>0.5455956697705323</v>
       </c>
       <c r="F50">
-        <v>0.6714771928459152</v>
+        <v>0.7038942061088712</v>
       </c>
       <c r="G50">
-        <v>-0.04271373793651367</v>
+        <v>-0.2653713507234592</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -1527,22 +1527,22 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>5.325819041892263</v>
+        <v>7.858711185153114</v>
       </c>
       <c r="C51">
-        <v>8.190190853725595</v>
+        <v>13.68671358760835</v>
       </c>
       <c r="D51">
-        <v>7.845782881665603</v>
+        <v>13.83792263620613</v>
       </c>
       <c r="E51">
-        <v>0.4810677099766353</v>
+        <v>0.5435632197871845</v>
       </c>
       <c r="F51">
-        <v>0.6711313185792461</v>
+        <v>0.7002805595211558</v>
       </c>
       <c r="G51">
-        <v>0.344407972059992</v>
+        <v>-0.1512090485977797</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -1550,22 +1550,22 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>5.460333267924816</v>
+        <v>7.931650115313854</v>
       </c>
       <c r="C52">
-        <v>8.46159300660549</v>
+        <v>13.66276824037254</v>
       </c>
       <c r="D52">
-        <v>8.090762761368559</v>
+        <v>13.8187232969058</v>
       </c>
       <c r="E52">
-        <v>0.48287760338781</v>
+        <v>0.5423433317998858</v>
       </c>
       <c r="F52">
-        <v>0.6738602463496844</v>
+        <v>0.6982394734809949</v>
       </c>
       <c r="G52">
-        <v>0.370830245236931</v>
+        <v>-0.1559550565332621</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -1573,22 +1573,22 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>5.161566111769502</v>
+        <v>7.82998835307921</v>
       </c>
       <c r="C53">
-        <v>8.555363010175155</v>
+        <v>13.60222989540548</v>
       </c>
       <c r="D53">
-        <v>8.375087111075691</v>
+        <v>13.80267723131894</v>
       </c>
       <c r="E53">
-        <v>0.4848525781692024</v>
+        <v>0.5411177260527267</v>
       </c>
       <c r="F53">
-        <v>0.6768974168325088</v>
+        <v>0.6961049612896849</v>
       </c>
       <c r="G53">
-        <v>0.1802758990994633</v>
+        <v>-0.2004473359134664</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -1596,22 +1596,22 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>4.897301898191372</v>
+        <v>7.741910468349206</v>
       </c>
       <c r="C54">
-        <v>8.673465699548824</v>
+        <v>13.82518189710272</v>
       </c>
       <c r="D54">
-        <v>8.311833163901117</v>
+        <v>13.65582452248281</v>
       </c>
       <c r="E54">
-        <v>0.4858369446584603</v>
+        <v>0.5395278479177142</v>
       </c>
       <c r="F54">
-        <v>0.6784228381195884</v>
+        <v>0.6933662957946991</v>
       </c>
       <c r="G54">
-        <v>0.3616325356477077</v>
+        <v>0.1693573746199171</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -1619,22 +1619,22 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>4.56235904028478</v>
+        <v>7.900428212003775</v>
       </c>
       <c r="C55">
-        <v>8.830034839691024</v>
+        <v>14.15503381484636</v>
       </c>
       <c r="D55">
-        <v>8.299543478312351</v>
+        <v>13.80500595438734</v>
       </c>
       <c r="E55">
-        <v>0.4877035348993727</v>
+        <v>0.5408539141884963</v>
       </c>
       <c r="F55">
-        <v>0.6815167357383446</v>
+        <v>0.6956699337387615</v>
       </c>
       <c r="G55">
-        <v>0.5304913613786724</v>
+        <v>0.3500278604590168</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -1642,22 +1642,22 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>4.568962098942847</v>
+        <v>7.945435720143569</v>
       </c>
       <c r="C56">
-        <v>8.907796274766287</v>
+        <v>14.37428470633225</v>
       </c>
       <c r="D56">
-        <v>8.295376796899959</v>
+        <v>14.21011722831322</v>
       </c>
       <c r="E56">
-        <v>0.4903015112504266</v>
+        <v>0.5435637985455978</v>
       </c>
       <c r="F56">
-        <v>0.6861179343651694</v>
+        <v>0.7005091325786611</v>
       </c>
       <c r="G56">
-        <v>0.6124194778663288</v>
+        <v>0.1641674780190385</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -1665,22 +1665,22 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>4.199502722885842</v>
+        <v>7.730607204464855</v>
       </c>
       <c r="C57">
-        <v>8.816800571489306</v>
+        <v>14.39830828112644</v>
       </c>
       <c r="D57">
-        <v>8.412904395336287</v>
+        <v>14.43187701791834</v>
       </c>
       <c r="E57">
-        <v>0.4930955887917166</v>
+        <v>0.5448607919204329</v>
       </c>
       <c r="F57">
-        <v>0.6915256196912345</v>
+        <v>0.7028329287813186</v>
       </c>
       <c r="G57">
-        <v>0.4038961761530189</v>
+        <v>-0.03356873679189576</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -1688,22 +1688,22 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>4.123044054871134</v>
+        <v>7.650830108850915</v>
       </c>
       <c r="C58">
-        <v>8.766531698909844</v>
+        <v>14.57073113567521</v>
       </c>
       <c r="D58">
-        <v>8.207270755768697</v>
+        <v>14.32270048176931</v>
       </c>
       <c r="E58">
-        <v>0.4949409751124677</v>
+        <v>0.5445940736800465</v>
       </c>
       <c r="F58">
-        <v>0.6951234445445627</v>
+        <v>0.70235040220144</v>
       </c>
       <c r="G58">
-        <v>0.5592609431411475</v>
+        <v>0.2480306539058983</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -1711,22 +1711,22 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>4.121272410437196</v>
+        <v>7.858750717926507</v>
       </c>
       <c r="C59">
-        <v>8.681985050918092</v>
+        <v>14.72852663944225</v>
       </c>
       <c r="D59">
-        <v>8.187395433885399</v>
+        <v>14.46706083496878</v>
       </c>
       <c r="E59">
-        <v>0.4972895929659926</v>
+        <v>0.5465115012400596</v>
       </c>
       <c r="F59">
-        <v>0.7000543367476612</v>
+        <v>0.7059216240195465</v>
       </c>
       <c r="G59">
-        <v>0.4945896170326929</v>
+        <v>0.2614658044734774</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -1734,22 +1734,22 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>4.155810379859843</v>
+        <v>7.825368533373076</v>
       </c>
       <c r="C60">
-        <v>8.76905858075687</v>
+        <v>14.43540384084531</v>
       </c>
       <c r="D60">
-        <v>8.17337498505163</v>
+        <v>14.76391595568194</v>
       </c>
       <c r="E60">
-        <v>0.4993288077461003</v>
+        <v>0.5485119316893603</v>
       </c>
       <c r="F60">
-        <v>0.7043901723033299</v>
+        <v>0.7097313719577025</v>
       </c>
       <c r="G60">
-        <v>0.5956835957052391</v>
+        <v>-0.3285121148366255</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -1757,22 +1757,22 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>4.229209109550798</v>
+        <v>7.811826940661698</v>
       </c>
       <c r="C61">
-        <v>8.681334688608166</v>
+        <v>14.64776895454112</v>
       </c>
       <c r="D61">
-        <v>8.307508016000895</v>
+        <v>14.44751857642985</v>
       </c>
       <c r="E61">
-        <v>0.5017837821144303</v>
+        <v>0.5459302368710404</v>
       </c>
       <c r="F61">
-        <v>0.7095618883763199</v>
+        <v>0.7048928725229517</v>
       </c>
       <c r="G61">
-        <v>0.3738266726072705</v>
+        <v>0.2002503781112743</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -1780,22 +1780,22 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>3.999747411472018</v>
+        <v>8.110881292996083</v>
       </c>
       <c r="C62">
-        <v>8.611443700254808</v>
+        <v>14.51929334263087</v>
       </c>
       <c r="D62">
-        <v>8.317121429746733</v>
+        <v>14.64440409080682</v>
       </c>
       <c r="E62">
-        <v>0.5033373348807201</v>
+        <v>0.5474972698787084</v>
       </c>
       <c r="F62">
-        <v>0.7128399963674625</v>
+        <v>0.7077835676002699</v>
       </c>
       <c r="G62">
-        <v>0.2943222705080757</v>
+        <v>-0.1251107481759455</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -1803,22 +1803,22 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>4.00270651630599</v>
+        <v>7.704951911663127</v>
       </c>
       <c r="C63">
-        <v>8.320930473393821</v>
+        <v>14.61206326546678</v>
       </c>
       <c r="D63">
-        <v>8.178785572684468</v>
+        <v>14.68266752791025</v>
       </c>
       <c r="E63">
-        <v>0.5045820853082965</v>
+        <v>0.5465199263655413</v>
       </c>
       <c r="F63">
-        <v>0.7153951065040542</v>
+        <v>0.7059509742672589</v>
       </c>
       <c r="G63">
-        <v>0.1421449007093525</v>
+        <v>-0.07060426244347262</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -1826,22 +1826,22 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>4.005394492434563</v>
+        <v>7.860580767484005</v>
       </c>
       <c r="C64">
-        <v>8.014191689110262</v>
+        <v>14.71304970725649</v>
       </c>
       <c r="D64">
-        <v>7.984908081412835</v>
+        <v>14.50691853374477</v>
       </c>
       <c r="E64">
-        <v>0.5051506290069627</v>
+        <v>0.5459472635740827</v>
       </c>
       <c r="F64">
-        <v>0.7166191793137912</v>
+        <v>0.7049258502696021</v>
       </c>
       <c r="G64">
-        <v>0.02928360769742788</v>
+        <v>0.2061311735117197</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -1849,22 +1849,22 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>4.04426097221094</v>
+        <v>7.859725531319284</v>
       </c>
       <c r="C65">
-        <v>7.735399238604606</v>
+        <v>14.73175465301275</v>
       </c>
       <c r="D65">
-        <v>7.76887329839936</v>
+        <v>14.7198717828182</v>
       </c>
       <c r="E65">
-        <v>0.5052678426943141</v>
+        <v>0.5475354943534853</v>
       </c>
       <c r="F65">
-        <v>0.7168628461774516</v>
+        <v>0.7079378520179402</v>
       </c>
       <c r="G65">
-        <v>-0.03347405979475315</v>
+        <v>0.01188287019455103</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -1872,22 +1872,22 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>4.276326826918968</v>
+        <v>7.7607883758125</v>
       </c>
       <c r="C66">
-        <v>8.205981640861813</v>
+        <v>14.96661756642138</v>
       </c>
       <c r="D66">
-        <v>7.586037933136395</v>
+        <v>14.73595519804556</v>
       </c>
       <c r="E66">
-        <v>0.5051337658795728</v>
+        <v>0.5476289006143991</v>
       </c>
       <c r="F66">
-        <v>0.7165945786456437</v>
+        <v>0.7081126852777776</v>
       </c>
       <c r="G66">
-        <v>0.619943707725418</v>
+        <v>0.2306623683758282</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -1895,22 +1895,22 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>4.191355245048815</v>
+        <v>7.603212721006281</v>
       </c>
       <c r="C67">
-        <v>8.229423076740554</v>
+        <v>14.92774066852474</v>
       </c>
       <c r="D67">
-        <v>8.090552581743186</v>
+        <v>14.91301111258038</v>
       </c>
       <c r="E67">
-        <v>0.5076409800216944</v>
+        <v>0.5494418435202372</v>
       </c>
       <c r="F67">
-        <v>0.7213900907303606</v>
+        <v>0.7115107466963732</v>
       </c>
       <c r="G67">
-        <v>0.1388704949973683</v>
+        <v>0.01472955594436165</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -1918,22 +1918,22 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>4.181265117812901</v>
+        <v>7.747454287333198</v>
       </c>
       <c r="C68">
-        <v>8.079504338595125</v>
+        <v>14.9133685986436</v>
       </c>
       <c r="D68">
-        <v>8.076194997309239</v>
+        <v>14.80293111423322</v>
       </c>
       <c r="E68">
-        <v>0.5082348356449192</v>
+        <v>0.549556156486791</v>
       </c>
       <c r="F68">
-        <v>0.7225296594627665</v>
+        <v>0.7117311983271156</v>
       </c>
       <c r="G68">
-        <v>0.003309341285886447</v>
+        <v>0.1104374844103777</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -1941,22 +1941,22 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>4.203020707650253</v>
+        <v>7.885350266877954</v>
       </c>
       <c r="C69">
-        <v>8.001672067154885</v>
+        <v>14.88650671905123</v>
       </c>
       <c r="D69">
-        <v>7.963024142067956</v>
+        <v>14.90306219742698</v>
       </c>
       <c r="E69">
-        <v>0.5082487062698755</v>
+        <v>0.5503958361731359</v>
       </c>
       <c r="F69">
-        <v>0.7225568934323133</v>
+        <v>0.713379780454478</v>
       </c>
       <c r="G69">
-        <v>0.03864792508692894</v>
+        <v>-0.01655547837575</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -1964,22 +1964,22 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>4.024673652434759</v>
+        <v>7.714828603999859</v>
       </c>
       <c r="C70">
-        <v>8.252778044100891</v>
+        <v>15.07508823667136</v>
       </c>
       <c r="D70">
-        <v>7.921020915403099</v>
+        <v>14.95511000341741</v>
       </c>
       <c r="E70">
-        <v>0.5084103034909173</v>
+        <v>0.5502675733612149</v>
       </c>
       <c r="F70">
-        <v>0.7228691495107309</v>
+        <v>0.7131328825031336</v>
       </c>
       <c r="G70">
-        <v>0.3317571286977916</v>
+        <v>0.1199782332539492</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -1987,22 +1987,22 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>3.76157933640713</v>
+        <v>7.557052883275574</v>
       </c>
       <c r="C71">
-        <v>8.777293956565506</v>
+        <v>15.21207548368912</v>
       </c>
       <c r="D71">
-        <v>8.03938405331666</v>
+        <v>15.02998487744722</v>
       </c>
       <c r="E71">
-        <v>0.5098046855727447</v>
+        <v>0.5512136437548235</v>
       </c>
       <c r="F71">
-        <v>0.7255237612605115</v>
+        <v>0.7149189392786084</v>
       </c>
       <c r="G71">
-        <v>0.7379099032488465</v>
+        <v>0.1820906062419034</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -2010,22 +2010,22 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>3.743895970062149</v>
+        <v>7.726501761714339</v>
       </c>
       <c r="C72">
-        <v>8.430943470248867</v>
+        <v>15.18378720449208</v>
       </c>
       <c r="D72">
-        <v>8.350429432396938</v>
+        <v>15.09332528958328</v>
       </c>
       <c r="E72">
-        <v>0.512774532118221</v>
+        <v>0.5526184415723783</v>
       </c>
       <c r="F72">
-        <v>0.7316135679085682</v>
+        <v>0.7176639712347741</v>
       </c>
       <c r="G72">
-        <v>0.08051403785192868</v>
+        <v>0.09046191490880773</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -2033,22 +2033,22 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>3.753835030550114</v>
+        <v>7.695846732056186</v>
       </c>
       <c r="C73">
-        <v>8.14075935721246</v>
+        <v>15.02798724035203</v>
       </c>
       <c r="D73">
-        <v>8.095059122346406</v>
+        <v>15.19284103357949</v>
       </c>
       <c r="E73">
-        <v>0.5130773920592955</v>
+        <v>0.5533020670472665</v>
       </c>
       <c r="F73">
-        <v>0.7323202632864246</v>
+        <v>0.7190400847127659</v>
       </c>
       <c r="G73">
-        <v>0.04570023486605379</v>
+        <v>-0.1648537932274614</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -2056,22 +2056,22 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <v>3.748926250820412</v>
+        <v>7.42059196946121</v>
       </c>
       <c r="C74">
-        <v>8.223952885981751</v>
+        <v>14.46949552428923</v>
       </c>
       <c r="D74">
-        <v>7.891429795956738</v>
+        <v>15.01643396229177</v>
       </c>
       <c r="E74">
-        <v>0.5132484889844414</v>
+        <v>0.5520283239234692</v>
       </c>
       <c r="F74">
-        <v>0.7327055593831574</v>
+        <v>0.7165369797965468</v>
       </c>
       <c r="G74">
-        <v>0.3325230900250125</v>
+        <v>-0.5469384380025382</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -2079,22 +2079,22 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <v>3.851913902716249</v>
+        <v>7.580938384679839</v>
       </c>
       <c r="C75">
-        <v>8.108888049538542</v>
+        <v>14.74737972681564</v>
       </c>
       <c r="D75">
-        <v>7.976808442985634</v>
+        <v>14.31414081422128</v>
       </c>
       <c r="E75">
-        <v>0.5144967258082441</v>
+        <v>0.5478191695327315</v>
       </c>
       <c r="F75">
-        <v>0.7354125498397677</v>
+        <v>0.7083175959289867</v>
       </c>
       <c r="G75">
-        <v>0.1320796065529084</v>
+        <v>0.4332389125943621</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -2102,22 +2102,22 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <v>3.718375704744504</v>
+        <v>7.635275004928535</v>
       </c>
       <c r="C76">
-        <v>7.975774955069995</v>
+        <v>14.67839258839172</v>
       </c>
       <c r="D76">
-        <v>7.955890436595862</v>
+        <v>14.71563141607057</v>
       </c>
       <c r="E76">
-        <v>0.5149918825124483</v>
+        <v>0.5510340587283873</v>
       </c>
       <c r="F76">
-        <v>0.7364987663012578</v>
+        <v>0.7145863444357188</v>
       </c>
       <c r="G76">
-        <v>0.01988451847413319</v>
+        <v>-0.037238827678852</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -2125,22 +2125,22 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>3.765696467298126</v>
+        <v>7.712396279347239</v>
       </c>
       <c r="C77">
-        <v>7.912821187876998</v>
+        <v>14.99608271092705</v>
       </c>
       <c r="D77">
-        <v>7.790652546611055</v>
+        <v>14.68605899093046</v>
       </c>
       <c r="E77">
-        <v>0.5150684759656077</v>
+        <v>0.5507517534702362</v>
       </c>
       <c r="F77">
-        <v>0.7366600076354834</v>
+        <v>0.7140371693033573</v>
       </c>
       <c r="G77">
-        <v>0.1221686412659428</v>
+        <v>0.3100237199965932</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -2148,22 +2148,22 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>3.180389717422949</v>
+        <v>7.760258833484087</v>
       </c>
       <c r="C78">
-        <v>7.724016992401133</v>
+        <v>15.33956494608492</v>
       </c>
       <c r="D78">
-        <v>7.778071266447913</v>
+        <v>15.04187428516289</v>
       </c>
       <c r="E78">
-        <v>0.5155227448731726</v>
+        <v>0.5531188698304611</v>
       </c>
       <c r="F78">
-        <v>0.7376343972247873</v>
+        <v>0.7185878191771808</v>
       </c>
       <c r="G78">
-        <v>-0.05405427404677976</v>
+        <v>0.2976906609220276</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -2171,22 +2171,22 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <v>3.10445079957182</v>
+        <v>7.810341299215828</v>
       </c>
       <c r="C79">
-        <v>8.218876678621371</v>
+        <v>15.08945185771805</v>
       </c>
       <c r="D79">
-        <v>7.333112750094283</v>
+        <v>15.40146575064284</v>
       </c>
       <c r="E79">
-        <v>0.5153191928843524</v>
+        <v>0.5554147781761526</v>
       </c>
       <c r="F79">
-        <v>0.7372066754198147</v>
+        <v>0.7230520129506381</v>
       </c>
       <c r="G79">
-        <v>0.885763928527088</v>
+        <v>-0.3120138929247922</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -2194,22 +2194,22 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>3.196366069113132</v>
+        <v>7.714121417101903</v>
       </c>
       <c r="C80">
-        <v>8.069697338725273</v>
+        <v>14.94893570115101</v>
       </c>
       <c r="D80">
-        <v>7.723770025413764</v>
+        <v>15.15730578262871</v>
       </c>
       <c r="E80">
-        <v>0.5181362673747041</v>
+        <v>0.5529934696074132</v>
       </c>
       <c r="F80">
-        <v>0.7440483310550139</v>
+        <v>0.7182658555760375</v>
       </c>
       <c r="G80">
-        <v>0.3459273133115088</v>
+        <v>-0.2083700814777067</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -2217,22 +2217,22 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>3.28918555015987</v>
+        <v>7.839800531002068</v>
       </c>
       <c r="C81">
-        <v>7.461333722743972</v>
+        <v>15.02695163159206</v>
       </c>
       <c r="D81">
-        <v>7.686773874810124</v>
+        <v>14.94361227896573</v>
       </c>
       <c r="E81">
-        <v>0.5192101816991077</v>
+        <v>0.551366028154527</v>
       </c>
       <c r="F81">
-        <v>0.7468914649828879</v>
+        <v>0.7151216652629908</v>
       </c>
       <c r="G81">
-        <v>-0.2254401520661515</v>
+        <v>0.08333935262633041</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -2240,22 +2240,22 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <v>3.505055102497661</v>
+        <v>7.873544777185263</v>
       </c>
       <c r="C82">
-        <v>7.820680899366089</v>
+        <v>14.52913404591119</v>
       </c>
       <c r="D82">
-        <v>7.264641039824083</v>
+        <v>15.09245958000716</v>
       </c>
       <c r="E82">
-        <v>0.5184895924464278</v>
+        <v>0.5520089180395091</v>
       </c>
       <c r="F82">
-        <v>0.7450722311877179</v>
+        <v>0.7163674998867774</v>
       </c>
       <c r="G82">
-        <v>0.5560398595420057</v>
+        <v>-0.5633255340959682</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -2263,22 +2263,22 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>3.822793541982587</v>
+        <v>8.331865811742666</v>
       </c>
       <c r="C83">
-        <v>7.897276289264807</v>
+        <v>14.31360835797216</v>
       </c>
       <c r="D83">
-        <v>7.683163650757249</v>
+        <v>14.59670388663635</v>
       </c>
       <c r="E83">
-        <v>0.5203185107177463</v>
+        <v>0.5475925582181765</v>
       </c>
       <c r="F83">
-        <v>0.7492210301429085</v>
+        <v>0.7079024343330765</v>
       </c>
       <c r="G83">
-        <v>0.2141126385075571</v>
+        <v>-0.2830955286641874</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -2286,22 +2286,22 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <v>3.921311245680601</v>
+        <v>8.29123999616874</v>
       </c>
       <c r="C84">
-        <v>7.904914064955572</v>
+        <v>14.47692725819359</v>
       </c>
       <c r="D84">
-        <v>7.92196867784138</v>
+        <v>14.61766070210414</v>
       </c>
       <c r="E84">
-        <v>0.5210689873138564</v>
+        <v>0.5453635928970181</v>
       </c>
       <c r="F84">
-        <v>0.7508955367651975</v>
+        <v>0.7037893014493165</v>
       </c>
       <c r="G84">
-        <v>-0.01705461288580779</v>
+        <v>-0.1407334439105519</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -2309,22 +2309,22 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>3.942355123601457</v>
+        <v>8.166458194706308</v>
       </c>
       <c r="C85">
-        <v>7.804661179719018</v>
+        <v>14.43402691204583</v>
       </c>
       <c r="D85">
-        <v>7.97771804150208</v>
+        <v>14.67156250730927</v>
       </c>
       <c r="E85">
-        <v>0.5210037910498555</v>
+        <v>0.544191020727131</v>
       </c>
       <c r="F85">
-        <v>0.7507608517752318</v>
+        <v>0.7017748980503122</v>
       </c>
       <c r="G85">
-        <v>-0.1730568617830626</v>
+        <v>-0.2375355952634362</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -2332,22 +2332,22 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <v>4.087845698032482</v>
+        <v>8.275606826016816</v>
       </c>
       <c r="C86">
-        <v>7.943279889635488</v>
+        <v>14.28185840710578</v>
       </c>
       <c r="D86">
-        <v>7.900063945736298</v>
+        <v>14.5078319118684</v>
       </c>
       <c r="E86">
-        <v>0.5203251812316034</v>
+        <v>0.542221556099169</v>
       </c>
       <c r="F86">
-        <v>0.7493928521544858</v>
+        <v>0.6983361125164518</v>
       </c>
       <c r="G86">
-        <v>0.04321594389919081</v>
+        <v>-0.225973504762619</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -2355,22 +2355,22 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>4.085282573743785</v>
+        <v>8.028156194906856</v>
       </c>
       <c r="C87">
-        <v>8.004931325286831</v>
+        <v>14.44307377863374</v>
       </c>
       <c r="D87">
-        <v>8.083021838031859</v>
+        <v>14.39889481243468</v>
       </c>
       <c r="E87">
-        <v>0.5204955538294557</v>
+        <v>0.5403761529194138</v>
       </c>
       <c r="F87">
-        <v>0.7497301379541808</v>
+        <v>0.6950744048672988</v>
       </c>
       <c r="G87">
-        <v>-0.07809051274502821</v>
+        <v>0.04417896619905726</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -2378,22 +2378,22 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>4.189399774455343</v>
+        <v>7.960256165847404</v>
       </c>
       <c r="C88">
-        <v>8.131720049915598</v>
+        <v>14.63951664427395</v>
       </c>
       <c r="D88">
-        <v>8.1216401533833</v>
+        <v>14.38928319612292</v>
       </c>
       <c r="E88">
-        <v>0.5201763318628737</v>
+        <v>0.5407417606736571</v>
       </c>
       <c r="F88">
-        <v>0.7491098431547218</v>
+        <v>0.695705362607126</v>
       </c>
       <c r="G88">
-        <v>0.01007989653229835</v>
+        <v>0.2502334481510307</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -2401,22 +2401,22 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <v>4.264488645928735</v>
+        <v>8.007309906604561</v>
       </c>
       <c r="C89">
-        <v>7.936139721558221</v>
+        <v>14.50292125973735</v>
       </c>
       <c r="D89">
-        <v>8.27160679417165</v>
+        <v>14.55813389860588</v>
       </c>
       <c r="E89">
-        <v>0.5202175110885222</v>
+        <v>0.5427506738806037</v>
       </c>
       <c r="F89">
-        <v>0.7491905320342289</v>
+        <v>0.6993195027606532</v>
       </c>
       <c r="G89">
-        <v>-0.3354670726134286</v>
+        <v>-0.05521263886853234</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -2424,22 +2424,22 @@
         <v>89</v>
       </c>
       <c r="B90">
-        <v>4.411830482149</v>
+        <v>7.981660341891258</v>
       </c>
       <c r="C90">
-        <v>7.941253366674488</v>
+        <v>14.45226440268646</v>
       </c>
       <c r="D90">
-        <v>8.136499884627284</v>
+        <v>14.47290675174485</v>
       </c>
       <c r="E90">
-        <v>0.5188121054101783</v>
+        <v>0.5423111671316178</v>
       </c>
       <c r="F90">
-        <v>0.7464626077137718</v>
+        <v>0.6985112164149631</v>
       </c>
       <c r="G90">
-        <v>-0.1952465179527962</v>
+        <v>-0.02064234905838802</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -2447,22 +2447,22 @@
         <v>90</v>
       </c>
       <c r="B91">
-        <v>4.114961419074521</v>
+        <v>8.164837467753403</v>
       </c>
       <c r="C91">
-        <v>8.027474403356658</v>
+        <v>14.36625666706722</v>
       </c>
       <c r="D91">
-        <v>8.200781349476632</v>
+        <v>14.41796639994822</v>
       </c>
       <c r="E91">
-        <v>0.5179794788512114</v>
+        <v>0.5421458774455069</v>
       </c>
       <c r="F91">
-        <v>0.7449131040671507</v>
+        <v>0.6982118420519532</v>
       </c>
       <c r="G91">
-        <v>-0.1733069461199737</v>
+        <v>-0.05170973288099923</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -2470,22 +2470,22 @@
         <v>91</v>
       </c>
       <c r="B92">
-        <v>4.353422817160328</v>
+        <v>8.39712829842864</v>
       </c>
       <c r="C92">
-        <v>8.169263913630289</v>
+        <v>14.24288081994439</v>
       </c>
       <c r="D92">
-        <v>8.097042136625756</v>
+        <v>14.44311740439782</v>
       </c>
       <c r="E92">
-        <v>0.5172148779835511</v>
+        <v>0.5417331479212808</v>
       </c>
       <c r="F92">
-        <v>0.7435368296978074</v>
+        <v>0.6974645193201647</v>
       </c>
       <c r="G92">
-        <v>0.07222177700453258</v>
+        <v>-0.2002365844534317</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -2493,22 +2493,22 @@
         <v>92</v>
       </c>
       <c r="B93">
-        <v>4.531961286233148</v>
+        <v>8.1310312129945</v>
       </c>
       <c r="C93">
-        <v>8.330710602553223</v>
+        <v>14.36470420904855</v>
       </c>
       <c r="D93">
-        <v>8.331833635380361</v>
+        <v>14.42820652788125</v>
       </c>
       <c r="E93">
-        <v>0.5175120678095418</v>
+        <v>0.5400982487541205</v>
       </c>
       <c r="F93">
-        <v>0.7441165881640762</v>
+        <v>0.6945878691537698</v>
       </c>
       <c r="G93">
-        <v>-0.001123032827138104</v>
+        <v>-0.06350231883270219</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -2516,22 +2516,22 @@
         <v>93</v>
       </c>
       <c r="B94">
-        <v>4.662455205461512</v>
+        <v>8.326682165098253</v>
       </c>
       <c r="C94">
-        <v>8.358007412505298</v>
+        <v>14.46671040116702</v>
       </c>
       <c r="D94">
-        <v>8.544266021232584</v>
+        <v>14.35177699631625</v>
       </c>
       <c r="E94">
-        <v>0.5175071787728077</v>
+        <v>0.5395650116356345</v>
       </c>
       <c r="F94">
-        <v>0.7441074138125277</v>
+        <v>0.6936834131948455</v>
       </c>
       <c r="G94">
-        <v>-0.1862586087272859</v>
+        <v>0.1149334048507757</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -2539,22 +2539,22 @@
         <v>94</v>
       </c>
       <c r="B95">
-        <v>4.560265919442341</v>
+        <v>8.417895700654476</v>
       </c>
       <c r="C95">
-        <v>8.061097779415764</v>
+        <v>14.59618746002937</v>
       </c>
       <c r="D95">
-        <v>8.615204822426611</v>
+        <v>14.55976923091247</v>
       </c>
       <c r="E95">
-        <v>0.5166630619688281</v>
+        <v>0.5404995387378919</v>
       </c>
       <c r="F95">
-        <v>0.7425557472459864</v>
+        <v>0.6953343975592657</v>
       </c>
       <c r="G95">
-        <v>-0.5541070430108466</v>
+        <v>0.03641822911690085</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -2562,22 +2562,22 @@
         <v>95</v>
       </c>
       <c r="B96">
-        <v>4.522563874226639</v>
+        <v>8.818047333987234</v>
       </c>
       <c r="C96">
-        <v>8.334826544362418</v>
+        <v>14.82975432302298</v>
       </c>
       <c r="D96">
-        <v>8.292821190789059</v>
+        <v>14.70934265580945</v>
       </c>
       <c r="E96">
-        <v>0.5140795627017593</v>
+        <v>0.5408027817567641</v>
       </c>
       <c r="F96">
-        <v>0.7379245164731804</v>
+        <v>0.6958612495332233</v>
       </c>
       <c r="G96">
-        <v>0.04200535357335866</v>
+        <v>0.1204116672135349</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -2585,22 +2585,22 @@
         <v>96</v>
       </c>
       <c r="B97">
-        <v>4.096838550554458</v>
+        <v>8.953331712602502</v>
       </c>
       <c r="C97">
-        <v>8.307349911071915</v>
+        <v>15.20053015212035</v>
       </c>
       <c r="D97">
-        <v>8.479119078214778</v>
+        <v>15.12327804101298</v>
       </c>
       <c r="E97">
-        <v>0.514271118284094</v>
+        <v>0.5418163946125095</v>
       </c>
       <c r="F97">
-        <v>0.7382631257355942</v>
+        <v>0.6976188008002467</v>
       </c>
       <c r="G97">
-        <v>-0.1717691671428625</v>
+        <v>0.07725211110737007</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -2608,22 +2608,22 @@
         <v>97</v>
       </c>
       <c r="B98">
-        <v>4.241419374738348</v>
+        <v>8.800902012888633</v>
       </c>
       <c r="C98">
-        <v>8.271750326921753</v>
+        <v>15.33268822532973</v>
       </c>
       <c r="D98">
-        <v>8.224819926664241</v>
+        <v>15.47875082921411</v>
       </c>
       <c r="E98">
-        <v>0.5134942812540677</v>
+        <v>0.5424976073849047</v>
       </c>
       <c r="F98">
-        <v>0.7368314595217889</v>
+        <v>0.6987644306289039</v>
       </c>
       <c r="G98">
-        <v>0.04693040025751216</v>
+        <v>-0.1460626038843813</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -2631,22 +2631,22 @@
         <v>98</v>
       </c>
       <c r="B99">
-        <v>4.435860298934845</v>
+        <v>8.86712902564183</v>
       </c>
       <c r="C99">
-        <v>8.399947095103098</v>
+        <v>15.24026826676218</v>
       </c>
       <c r="D99">
-        <v>8.276870826014839</v>
+        <v>15.44285401063047</v>
       </c>
       <c r="E99">
-        <v>0.5136865475270357</v>
+        <v>0.5411898604415214</v>
       </c>
       <c r="F99">
-        <v>0.7372213267781946</v>
+        <v>0.6965442016144622</v>
       </c>
       <c r="G99">
-        <v>0.1230762690882585</v>
+        <v>-0.2025857438682888</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -2654,22 +2654,22 @@
         <v>99</v>
       </c>
       <c r="B100">
-        <v>4.301690293368822</v>
+        <v>8.811482210597919</v>
       </c>
       <c r="C100">
-        <v>8.420631632772929</v>
+        <v>15.66751685876251</v>
       </c>
       <c r="D100">
-        <v>8.4821291217928</v>
+        <v>15.35117219904867</v>
       </c>
       <c r="E100">
-        <v>0.5142085655993172</v>
+        <v>0.5394069231605284</v>
       </c>
       <c r="F100">
-        <v>0.7382393829472618</v>
+        <v>0.6934380175648333</v>
       </c>
       <c r="G100">
-        <v>-0.06149748901987095</v>
+        <v>0.31634465971384</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -2677,22 +2677,22 @@
         <v>100</v>
       </c>
       <c r="B101">
-        <v>4.517261771309791</v>
+        <v>8.96208227066767</v>
       </c>
       <c r="C101">
-        <v>8.205000444085456</v>
+        <v>15.8534001892278</v>
       </c>
       <c r="D101">
-        <v>8.422884526251819</v>
+        <v>15.71767903267183</v>
       </c>
       <c r="E101">
-        <v>0.5139357713292897</v>
+        <v>0.5422119920747838</v>
       </c>
       <c r="F101">
-        <v>0.7377228072930132</v>
+        <v>0.6982591950436298</v>
       </c>
       <c r="G101">
-        <v>-0.2178840821663623</v>
+        <v>0.1357211565559702</v>
       </c>
     </row>
   </sheetData>

</xml_diff>